<commit_message>
some changes unknown on Sat.
Maybe has some changes on Sat
</commit_message>
<xml_diff>
--- a/Table for I-V.xlsx
+++ b/Table for I-V.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlbertCielstian\Documents\.All.PDF\Chemistry\Chemistry Bsc Y3\1. Courses\-- Practical Chemistry 3 for BSc Chemistry 2022-2023\Physical - P3-5 DSSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlbertCielstian\Documents\GitHub\y3_DSSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA677171-FF7A-4894-B3C8-AE8F78E7D4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E76FEA-4CE4-46B6-A7BB-94B9749353CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54075" yWindow="5100" windowWidth="12255" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="16200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Opti. Power</t>
   </si>
   <si>
-    <t>Light power</t>
-  </si>
-  <si>
     <t>P Conv. Effi.</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>SC5-BlueB</t>
+  </si>
+  <si>
+    <t>Light power22222222222222</t>
   </si>
 </sst>
 </file>
@@ -406,17 +406,17 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -428,10 +428,10 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -504,7 +504,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -521,7 +521,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Undate on the jupyter notebook and excel
Ploting IV Curves
Calculate the parameter for this experiment, V_OC and I_SC and etc.
</commit_message>
<xml_diff>
--- a/Table for I-V.xlsx
+++ b/Table for I-V.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlbertCielstian\Documents\GitHub\y3_DSSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E76FEA-4CE4-46B6-A7BB-94B9749353CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0438BBC-04CF-4B75-88DB-35E6FDC89F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="16200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54450" yWindow="7095" windowWidth="12765" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>V_OC</t>
   </si>
   <si>
-    <t>I_IS</t>
-  </si>
-  <si>
     <t>Opti. Power</t>
   </si>
   <si>
@@ -74,14 +71,17 @@
     <t>SC5-BlueB</t>
   </si>
   <si>
-    <t>Light power22222222222222</t>
+    <t>Light power</t>
+  </si>
+  <si>
+    <t>I_SC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,10 +137,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,42 +437,38 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="E2">
-        <f>C2*D2</f>
-        <v>0</v>
-      </c>
       <c r="F2" t="e">
         <f>E2/B2</f>
         <v>#DIV/0!</v>
@@ -455,33 +482,37 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E7" si="0">C3*D3</f>
-        <v>0</v>
-      </c>
-      <c r="F3" t="e">
-        <f t="shared" ref="F3:F7" si="1">E3/B3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
-        <f t="shared" ref="G3:G7" si="2">E3/(C3*D3)</f>
-        <v>#DIV/0!</v>
+      <c r="B3">
+        <v>1.03</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.43555094523216797</v>
+      </c>
+      <c r="D3">
+        <v>5.95059E-4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.4060661561480001E-4</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="0">E3/B3</f>
+        <v>1.3651127729592233E-4</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="1">E3/(C3*D3)</f>
+        <v>0.54250877381304796</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="F4" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
-        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -489,51 +520,69 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="B5" s="4">
+        <v>1.03</v>
+      </c>
+      <c r="C5" s="5">
+        <v>-6.91728065845537E-2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1.8923982E-7</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" t="e">
+      <c r="G5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1.03</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-5.0010018548270398E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>3.1655643999999998E-6</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" t="e">
+      <c r="G6">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1.03</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.13678308581395601</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.118747E-5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>5.5025570662209095E-7</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" t="e">
+        <v>5.3422884138067081E-7</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.35958392977520237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>